<commit_message>
Atualizar casos de uso
</commit_message>
<xml_diff>
--- a/Casos de Uso e atores.xlsx
+++ b/Casos de Uso e atores.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IPG\2018-2019\Eng-Software2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1011418\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD26BC9F-6E16-4D3D-879B-9B069CD351AD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{D4609021-9C50-4950-AF2A-8B9582BB7A93}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
   <si>
     <t>Casos de uso</t>
   </si>
@@ -86,11 +85,14 @@
   <si>
     <t>Folha de Impressao</t>
   </si>
+  <si>
+    <t>instalar visio</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -486,11 +488,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C68DF796-CC74-404C-A4BB-7CB603DB02D1}">
-  <dimension ref="A1:K8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,6 +639,11 @@
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F8" s="7"/>
     </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>

</xml_diff>